<commit_message>
Update 1.3.6: Hidden Import and Invoice Output Out Of Project
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта СИП.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта СИП.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87075916-01B5-4400-942A-1581F9B9B74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Импорт" sheetId="1" r:id="rId1"/>
+    <sheet name="СИП" sheetId="1" r:id="rId1"/>
     <sheet name="Супервайзеры" sheetId="2" r:id="rId2"/>
+    <sheet name="Бригады" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Имя</t>
   </si>
@@ -46,11 +48,11 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -62,63 +64,31 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>Супервайзер</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
+    <t>Кол-во фидеров</t>
   </si>
   <si>
-    <r>
-      <t>Кол-во фидеров</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
+    <t>Супервайзер</t>
   </si>
   <si>
-    <t>Сиаваш</t>
-  </si>
-  <si>
-    <t>Шахзод</t>
-  </si>
-  <si>
-    <t>Мурод</t>
+    <t>Бригада</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,7 +97,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,7 +105,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,7 +113,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -173,14 +143,14 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -193,7 +163,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -457,15 +427,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
@@ -483,32 +453,31 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B159" xr:uid="{97E180B8-70D3-40D7-9813-50FDDD79F612}">
       <formula1>"  В ожидании, Идет работа, Работа завершена,   Сдано заказчику,"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E126 D2:D1048576" xr:uid="{369879D8-D174-4EAD-B927-0696E229D932}">
-      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BEF7AA8-B587-4114-8370-3FF93C5AD676}">
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7C8ECB0-E6E9-4C08-A6CF-329A40512207}">
           <x14:formula1>
-            <xm:f>Супервайзеры!$A$2:$A$220</xm:f>
+            <xm:f>Супервайзеры!A2:A1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>E127:E131</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F8D1B3DC-4DE7-4F45-ACEC-014DB6ED8F00}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9417DCA-4F8C-4F6D-8912-D2AA217FC140}">
           <x14:formula1>
-            <xm:f>Супервайзеры!$A$2:$A$58</xm:f>
+            <xm:f>Бригады!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C157</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -520,30 +489,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63442B1F-92B5-41D0-B08A-E102BBCB0DA7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1.5.12: Changes to SIP, Import template MJD fix
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта СИП.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта СИП.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\TGEM\tgem-backend\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51D8035-6A9D-47C8-ABF0-D4BA8373114C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="СИП" sheetId="1" r:id="rId1"/>
-    <sheet name="Супервайзеры" sheetId="2" r:id="rId2"/>
-    <sheet name="Бригады" sheetId="3" r:id="rId3"/>
+    <sheet name="ТП" sheetId="4" r:id="rId2"/>
+    <sheet name="Супервайзеры" sheetId="2" r:id="rId3"/>
+    <sheet name="Бригады" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Имя</t>
   </si>
@@ -96,11 +96,17 @@
       <t>*</t>
     </r>
   </si>
+  <si>
+    <t>Питается от ТП</t>
+  </si>
+  <si>
+    <t>Наименование ТП</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +166,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,23 +443,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -468,30 +475,39 @@
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B159" xr:uid="{97E180B8-70D3-40D7-9813-50FDDD79F612}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B159">
       <formula1>"  В ожидании, Идет работа, Работа завершена,   Сдано заказчику,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7C8ECB0-E6E9-4C08-A6CF-329A40512207}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Супервайзеры!A2:A1048576</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9417DCA-4F8C-4F6D-8912-D2AA217FC140}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Бригады!$A$2:$A$1048576</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ТП!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -499,16 +515,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A1048539" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,17 +558,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63442B1F-92B5-41D0-B08A-E102BBCB0DA7}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>